<commit_message>
DONE: Test 300_1 first (again)
</commit_message>
<xml_diff>
--- a/Esercizio 1/Res/res con grafici.xlsx
+++ b/Esercizio 1/Res/res con grafici.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leobartowski/Desktop/ASSSC/Esercizio 1/Res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E00B77C-7569-9E4E-8E79-D3019D4220CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F0B494-55B4-0346-986D-DD5AD418FD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37140" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3632,7 +3632,7 @@
   <dimension ref="A1:R995"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
DONE: Added final thesis
</commit_message>
<xml_diff>
--- a/Esercizio 1/Res/res con grafici.xlsx
+++ b/Esercizio 1/Res/res con grafici.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leobartowski/Desktop/ASSSC/Esercizio 1/Res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F0B494-55B4-0346-986D-DD5AD418FD8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2B1226-E798-0541-8C4E-A519CB595F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37140" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]\.mm\.ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -140,8 +140,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,18 +157,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF73FB79"/>
-        <bgColor rgb="FFCC0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -179,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -198,21 +191,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -256,11 +244,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -270,7 +258,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>THROUGHPUT</a:t>
+              <a:t>POTENZA</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -288,11 +276,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -314,7 +302,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -323,7 +311,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -371,34 +371,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>50.0717133333333</c:v>
+                  <c:v>13.33333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.05314</c:v>
+                  <c:v>3130.0558679999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>149.94499999999999</c:v>
+                  <c:v>4630.4411899999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>185.001</c:v>
+                  <c:v>7931.4944450000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>187.465826666667</c:v>
+                  <c:v>9220.9176910000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>172.50650999999999</c:v>
+                  <c:v>6230.9622339999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>166.11147333333301</c:v>
+                  <c:v>3199.6389859999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>156.17406</c:v>
+                  <c:v>2505.2842620000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>137.03200666666601</c:v>
+                  <c:v>2210.0177309999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>137.03200666666601</c:v>
+                  <c:v>1850.151396</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,21 +418,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:dropLines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="35000"/>
-                  <a:lumOff val="65000"/>
-                  <a:alpha val="33000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:dropLines>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="95196539"/>
         <c:axId val="1731733690"/>
@@ -451,9 +437,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
+                      <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -480,9 +466,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
+                    <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -504,7 +490,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="dk1">
+              <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -518,9 +504,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -547,6 +533,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -554,9 +554,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
+                      <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -583,9 +583,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
+                    <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -615,9 +615,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -635,19 +635,7 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -660,11 +648,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
+        <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -712,11 +700,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -726,7 +714,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>ELAPSED</a:t>
+              <a:t>ELAPSED TIME</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -744,11 +732,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -770,7 +758,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -779,7 +767,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -822,33 +822,39 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio1!$B$4:$B$11</c:f>
+              <c:f>Foglio1!$B$4:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>35.422555555555498</c:v>
+                  <c:v>14.33333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.079944444444401</c:v>
+                  <c:v>10.33333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.250172279648702</c:v>
+                  <c:v>12.33333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.153267934686298</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>117.23497717544601</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>157.20432634173099</c:v>
+                  <c:v>31.666666670000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>136.00652195614299</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>175.51848410921301</c:v>
+                  <c:v>67.333333330000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72.333333330000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>78.666666669999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -868,21 +874,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:dropLines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="35000"/>
-                  <a:lumOff val="65000"/>
-                  <a:alpha val="33000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:dropLines>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="2139242496"/>
         <c:axId val="1183346998"/>
@@ -901,9 +893,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
+                      <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -930,9 +922,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
+                    <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -954,7 +946,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="dk1">
+              <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -968,9 +960,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -997,6 +989,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1004,9 +1010,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
+                      <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -1033,9 +1039,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
+                    <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -1065,9 +1071,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -1085,19 +1091,7 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1110,11 +1104,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
+        <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1162,11 +1156,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1176,7 +1170,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>POTENZA</a:t>
+              <a:t>THROUGHPUT</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1194,11 +1188,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1220,7 +1214,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1229,7 +1223,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1277,34 +1283,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1413.55451485713</c:v>
+                  <c:v>12.33333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2560.2170479600959</c:v>
+                  <c:v>100.01846</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6739.0489437759716</c:v>
+                  <c:v>141.66698</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5262.6970654257875</c:v>
+                  <c:v>198.39012500000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1599.0605464623259</c:v>
+                  <c:v>247.22620330000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1097.3394563264442</c:v>
+                  <c:v>266.30547000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1221.3493216663369</c:v>
+                  <c:v>277.39233999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>889.78696911958116</c:v>
+                  <c:v>255.1759533</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>724.67452924494637</c:v>
+                  <c:v>248.42789329999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>630.16351772483324</c:v>
+                  <c:v>231.76929000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1324,21 +1330,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:dropLines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="35000"/>
-                  <a:lumOff val="65000"/>
-                  <a:alpha val="33000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:dropLines>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="95196539"/>
         <c:axId val="1731733690"/>
@@ -1357,9 +1349,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
+                      <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -1386,9 +1378,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
+                    <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -1410,7 +1402,7 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="dk1">
+              <a:schemeClr val="tx1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -1424,9 +1416,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -1453,6 +1445,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1460,9 +1466,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
+                      <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
@@ -1489,9 +1495,9 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="dk1">
+                    <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
@@ -1521,9 +1527,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="dk1">
+                  <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
@@ -1541,19 +1547,7 @@
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="lt1"/>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1566,11 +1560,11 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="dk1">
+        <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1718,25 +1712,25 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -1744,7 +1738,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1752,22 +1746,22 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -1775,16 +1769,16 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1818,60 +1812,36 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1883,34 +1853,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1926,19 +1892,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1953,13 +1921,13 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -1972,15 +1940,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
-            <a:alpha val="33000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1992,16 +1959,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -2010,24 +1978,31 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -2036,16 +2011,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2054,133 +2030,109 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2189,13 +2141,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2204,7 +2157,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2224,9 +2177,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2237,44 +2190,50 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2282,7 +2241,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2290,22 +2249,22 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2313,16 +2272,16 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2356,60 +2315,36 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2421,34 +2356,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2464,19 +2395,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2491,13 +2424,13 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -2510,15 +2443,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
-            <a:alpha val="33000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2530,16 +2462,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -2548,24 +2481,31 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -2574,16 +2514,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2592,133 +2533,109 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2727,13 +2644,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2742,7 +2660,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2762,9 +2680,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2775,44 +2693,50 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -2820,7 +2744,7 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2828,22 +2752,22 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="bg1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2851,16 +2775,16 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2894,60 +2818,36 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2959,34 +2859,30 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -3002,19 +2898,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -3029,13 +2927,13 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
@@ -3048,15 +2946,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="dk1">
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
-            <a:alpha val="33000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -3068,16 +2965,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:errorBar>
@@ -3086,24 +2984,31 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMajor>
@@ -3112,16 +3017,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -3130,133 +3036,109 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1"/>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3265,13 +3147,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3280,7 +3163,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
@@ -3300,9 +3183,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3313,20 +3196,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
+      <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3367,9 +3256,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>306036</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>74462</xdr:rowOff>
+      <xdr:colOff>224756</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>125262</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5181600" cy="2857500"/>
     <xdr:graphicFrame macro="">
@@ -3397,10 +3286,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>592667</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>13547</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>33867</xdr:rowOff>
+      <xdr:rowOff>13547</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5181600" cy="2857500"/>
     <xdr:graphicFrame macro="">
@@ -3631,8 +3520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R995"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="157" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1"/>
@@ -3667,24 +3556,24 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1">
       <c r="A4" s="5">
         <v>100</v>
       </c>
-      <c r="B4" s="5">
-        <v>35.422555555555498</v>
-      </c>
-      <c r="C4" s="6">
-        <v>50.0717133333333</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1413.55451485713</v>
+      <c r="B4" s="8">
+        <v>14.33333333</v>
+      </c>
+      <c r="C4" s="8">
+        <v>13.33333333</v>
+      </c>
+      <c r="D4" s="8">
+        <v>12.33333333</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -3694,135 +3583,126 @@
       <c r="A5" s="5">
         <v>200</v>
       </c>
-      <c r="B5" s="6">
-        <v>39.079944444444401</v>
-      </c>
-      <c r="C5" s="6">
-        <v>100.05314</v>
-      </c>
-      <c r="D5" s="6">
-        <f t="shared" ref="D5:D13" si="0">C5/(B5/1000)</f>
-        <v>2560.2170479600959</v>
+      <c r="B5" s="8">
+        <v>10.33333333</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3130.0558679999999</v>
+      </c>
+      <c r="D5" s="8">
+        <v>100.01846</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A6" s="8">
+    <row r="6" spans="1:18" s="11" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A6" s="9">
         <v>300</v>
       </c>
-      <c r="B6" s="9">
-        <v>22.250172279648702</v>
-      </c>
-      <c r="C6" s="9">
-        <v>149.94499999999999</v>
-      </c>
-      <c r="D6" s="9">
-        <f t="shared" si="0"/>
-        <v>6739.0489437759716</v>
+      <c r="B6" s="10">
+        <v>12.33333333</v>
+      </c>
+      <c r="C6" s="10">
+        <v>4630.4411899999996</v>
+      </c>
+      <c r="D6" s="10">
+        <v>141.66698</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1">
+    <row r="7" spans="1:18" ht="14" customHeight="1">
       <c r="A7" s="5">
         <v>400</v>
       </c>
-      <c r="B7" s="6">
-        <v>35.153267934686298</v>
-      </c>
-      <c r="C7" s="6">
-        <v>185.001</v>
-      </c>
-      <c r="D7" s="6">
-        <f t="shared" si="0"/>
-        <v>5262.6970654257875</v>
+      <c r="B7" s="8">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8">
+        <v>7931.4944450000003</v>
+      </c>
+      <c r="D7" s="8">
+        <v>198.39012500000001</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A8" s="10">
+    <row r="8" spans="1:18" s="11" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A8" s="9">
         <v>500</v>
       </c>
-      <c r="B8" s="11">
-        <v>117.23497717544601</v>
-      </c>
-      <c r="C8" s="12">
-        <v>187.465826666667</v>
-      </c>
-      <c r="D8" s="11">
-        <f t="shared" si="0"/>
-        <v>1599.0605464623259</v>
+      <c r="B8" s="10">
+        <v>16</v>
+      </c>
+      <c r="C8" s="10">
+        <v>9220.9176910000006</v>
+      </c>
+      <c r="D8" s="10">
+        <v>247.22620330000001</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1">
       <c r="A9" s="5">
         <v>600</v>
       </c>
-      <c r="B9" s="6">
-        <v>157.20432634173099</v>
-      </c>
-      <c r="C9" s="6">
-        <v>172.50650999999999</v>
-      </c>
-      <c r="D9" s="6">
-        <f t="shared" si="0"/>
-        <v>1097.3394563264442</v>
+      <c r="B9" s="8">
+        <v>31.666666670000001</v>
+      </c>
+      <c r="C9" s="8">
+        <v>6230.9622339999996</v>
+      </c>
+      <c r="D9" s="8">
+        <v>266.30547000000001</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1">
       <c r="A10" s="5">
         <v>700</v>
       </c>
-      <c r="B10" s="6">
-        <v>136.00652195614299</v>
-      </c>
-      <c r="C10" s="6">
-        <v>166.11147333333301</v>
-      </c>
-      <c r="D10" s="6">
-        <f t="shared" si="0"/>
-        <v>1221.3493216663369</v>
+      <c r="B10" s="8">
+        <v>57</v>
+      </c>
+      <c r="C10" s="8">
+        <v>3199.6389859999999</v>
+      </c>
+      <c r="D10" s="8">
+        <v>277.39233999999999</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1">
       <c r="A11" s="5">
         <v>800</v>
       </c>
-      <c r="B11" s="6">
-        <v>175.51848410921301</v>
-      </c>
-      <c r="C11" s="6">
-        <v>156.17406</v>
-      </c>
-      <c r="D11" s="6">
-        <f t="shared" si="0"/>
-        <v>889.78696911958116</v>
+      <c r="B11" s="8">
+        <v>67.333333330000002</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2505.2842620000001</v>
+      </c>
+      <c r="D11" s="8">
+        <v>255.1759533</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1">
       <c r="A12" s="5">
         <v>900</v>
       </c>
-      <c r="B12" s="6">
-        <v>189.094553674244</v>
-      </c>
-      <c r="C12" s="6">
-        <v>137.03200666666601</v>
-      </c>
-      <c r="D12" s="6">
-        <f t="shared" si="0"/>
-        <v>724.67452924494637</v>
+      <c r="B12" s="8">
+        <v>72.333333330000002</v>
+      </c>
+      <c r="C12" s="8">
+        <v>2210.0177309999999</v>
+      </c>
+      <c r="D12" s="8">
+        <v>248.42789329999999</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1">
       <c r="A13" s="5">
         <v>1000</v>
       </c>
-      <c r="B13" s="6">
-        <v>217.45468090791999</v>
-      </c>
-      <c r="C13" s="6">
-        <v>137.03200666666601</v>
-      </c>
-      <c r="D13" s="6">
-        <f t="shared" si="0"/>
-        <v>630.16351772483324</v>
+      <c r="B13" s="8">
+        <v>78.666666669999998</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1850.151396</v>
+      </c>
+      <c r="D13" s="8">
+        <v>231.76929000000001</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1"/>
@@ -3837,7 +3717,7 @@
         <v>125.00014</v>
       </c>
       <c r="D15" s="6">
-        <f t="shared" ref="D15" si="1">C15/(B15/1000)</f>
+        <f t="shared" ref="D15" si="0">C15/(B15/1000)</f>
         <v>3307.0022347928448</v>
       </c>
     </row>
@@ -3862,22 +3742,26 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1"/>
     <row r="32" spans="1:2" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="33" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="34" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="35" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="36" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="37" spans="4:4" ht="15.75" customHeight="1">
+      <c r="D37" s="8">
+        <v>266.30547000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="39" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="40" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="41" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="42" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="43" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="44" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="45" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="46" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="47" spans="4:4" ht="15.75" customHeight="1"/>
+    <row r="48" spans="4:4" ht="15.75" customHeight="1"/>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>

</xml_diff>